<commit_message>
Touch valid template to recommit.
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Library_capture_v3_14_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Library_capture_v3_14_0.xlsx
@@ -679,7 +679,7 @@
       <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
@@ -9077,7 +9077,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.3"/>
@@ -17961,7 +17961,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>

</xml_diff>